<commit_message>
Full positive set of addition tests is added
test data was moved todataprovider;
test class was renamed to Adding ComputerHappyPath
</commit_message>
<xml_diff>
--- a/ComputerDatabase_TestCases.xlsx
+++ b/ComputerDatabase_TestCases.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="87">
   <si>
     <t>Test Case Id</t>
   </si>
@@ -354,6 +354,21 @@
   </si>
   <si>
     <t>Automation test name</t>
+  </si>
+  <si>
+    <t>\src\test\java\me\manzhos\tests\AddingComputerHappyPathTest</t>
+  </si>
+  <si>
+    <t>addComputerWithFieldsFromDataProviderTest (case 1 in dataprovider)</t>
+  </si>
+  <si>
+    <t>addComputerWithFieldsFromDataProviderTest (case 2 in dataprovider)</t>
+  </si>
+  <si>
+    <t>addComputerWithFieldsFromDataProviderTest (case 3 in dataprovider)</t>
+  </si>
+  <si>
+    <t>addComputerWithFieldsFromDataProviderTest (case 4 in dataprovider)</t>
   </si>
 </sst>
 </file>
@@ -534,78 +549,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -621,29 +597,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -653,6 +614,60 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -938,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -952,521 +967,521 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="13" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="14" t="s">
+      <c r="A7" s="41"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="14" t="s">
+      <c r="A9" s="41"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="14" t="s">
+      <c r="A11" s="41"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="6" t="s">
+      <c r="A13" s="43"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="4" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="6" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="6" t="s">
+      <c r="A16" s="39"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="6" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="6" t="s">
+      <c r="A17" s="39"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="6" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="6" t="s">
+      <c r="A18" s="39"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="6" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="6" t="s">
+      <c r="A19" s="39"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="6" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="23"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="6" t="s">
+      <c r="A20" s="39"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="6" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="23"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="6" t="s">
+      <c r="A21" s="39"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="4" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="23"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="6" t="s">
+      <c r="A22" s="39"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="6" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="23"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="6" t="s">
+      <c r="A23" s="39"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="E23" s="6" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="23"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="6" t="s">
+      <c r="A24" s="39"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E24" s="6" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="32" t="s">
+      <c r="A25" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="6" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="33"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="6" t="s">
+      <c r="A26" s="30"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="6" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="33"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="6" t="s">
+      <c r="A27" s="30"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E27" s="6" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="33"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="6" t="s">
+      <c r="A28" s="30"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E28" s="6" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="33"/>
-      <c r="B29" s="24"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="6" t="s">
+      <c r="A29" s="30"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E29" s="6" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="33"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="6" t="s">
+      <c r="A30" s="30"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E30" s="6" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="33"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="6" t="s">
+      <c r="A31" s="30"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="E31" s="6" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="33"/>
-      <c r="B32" s="24"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="6" t="s">
+      <c r="A32" s="30"/>
+      <c r="B32" s="33"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E32" s="8" t="s">
+      <c r="E32" s="6" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="39"/>
-      <c r="B33" s="16"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="6" t="s">
+      <c r="A33" s="31"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E33" s="8" t="s">
+      <c r="E33" s="6" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A34" s="30" t="s">
+      <c r="A34" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="21" t="s">
+      <c r="B34" s="12" t="s">
         <v>29</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D34" s="28" t="s">
+      <c r="D34" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="E34" s="29" t="s">
+      <c r="E34" s="16" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A35" s="34" t="s">
+      <c r="A35" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="38" t="s">
+      <c r="C35" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="D35" s="31" t="s">
+      <c r="D35" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="E35" s="37" t="s">
+      <c r="E35" s="20" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="35" t="s">
+      <c r="A36" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="B36" s="36" t="s">
+      <c r="B36" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="C36" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="D36" s="29" t="s">
+      <c r="D36" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="E36" s="29" t="s">
+      <c r="E36" s="16" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="135" x14ac:dyDescent="0.25">
-      <c r="A37" s="35"/>
-      <c r="B37" s="36"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="29" t="s">
+      <c r="A37" s="26"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="E37" s="29" t="s">
+      <c r="E37" s="16" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A38" s="40" t="s">
+      <c r="A38" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="B38" s="21" t="s">
+      <c r="B38" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C38" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D38" s="29" t="s">
+      <c r="D38" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="E38" s="29" t="s">
+      <c r="E38" s="16" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A39" s="35" t="s">
+      <c r="A39" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="B39" s="36" t="s">
+      <c r="B39" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="C39" s="9" t="s">
+      <c r="C39" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="D39" s="29" t="s">
+      <c r="D39" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="E39" s="29" t="s">
+      <c r="E39" s="16" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="35"/>
-      <c r="B40" s="36"/>
-      <c r="C40" s="9"/>
+      <c r="A40" s="26"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="28"/>
       <c r="D40" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E40" s="29" t="s">
+      <c r="E40" s="16" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="41"/>
-      <c r="B41" s="42"/>
-      <c r="C41" s="41"/>
-      <c r="D41" s="41"/>
-      <c r="E41" s="41"/>
+      <c r="A41" s="23"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="23"/>
     </row>
   </sheetData>
   <autoFilter ref="A5:E9"/>
   <mergeCells count="24">
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A25:A33"/>
+    <mergeCell ref="B25:B33"/>
+    <mergeCell ref="C25:C33"/>
+    <mergeCell ref="A15:A24"/>
+    <mergeCell ref="B15:B24"/>
+    <mergeCell ref="C15:C24"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="C39:C40"/>
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="B36:B37"/>
     <mergeCell ref="C36:C37"/>
-    <mergeCell ref="A25:A33"/>
-    <mergeCell ref="B25:B33"/>
-    <mergeCell ref="C25:C33"/>
-    <mergeCell ref="A15:A24"/>
-    <mergeCell ref="B15:B24"/>
-    <mergeCell ref="C15:C24"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="A8:A9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
@@ -1481,24 +1496,24 @@
   <dimension ref="C2:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="25.42578125" customWidth="1"/>
-    <col min="4" max="4" width="47" customWidth="1"/>
-    <col min="5" max="5" width="37.7109375" customWidth="1"/>
+    <col min="4" max="4" width="62.42578125" customWidth="1"/>
+    <col min="5" max="5" width="64.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="43" t="s">
+      <c r="D2" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="E2" s="43" t="s">
+      <c r="E2" s="25" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1506,29 +1521,45 @@
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">

</xml_diff>

<commit_message>
Addition test were expanded
Tests on Happy and Unhappy paths were added;
Cancel test was added
</commit_message>
<xml_diff>
--- a/ComputerDatabase_TestCases.xlsx
+++ b/ComputerDatabase_TestCases.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="92">
   <si>
     <t>Test Case Id</t>
   </si>
@@ -245,13 +245,6 @@
   </si>
   <si>
     <t>"Discontinued date" field is highlighted with red</t>
-  </si>
-  <si>
-    <t>Discontinued date" field is highlighted with red</t>
-  </si>
-  <si>
-    <t>1. "Introduced date" field is highlighted with red
-2. Discontinued date" field is highlighted with red</t>
   </si>
   <si>
     <t>1. Input "Incorrect dates" to "Computer name" field
@@ -356,9 +349,6 @@
     <t>Automation test name</t>
   </si>
   <si>
-    <t>\src\test\java\me\manzhos\tests\AddingComputerHappyPathTest</t>
-  </si>
-  <si>
     <t>addComputerWithFieldsFromDataProviderTest (case 1 in dataprovider)</t>
   </si>
   <si>
@@ -369,6 +359,31 @@
   </si>
   <si>
     <t>addComputerWithFieldsFromDataProviderTest (case 4 in dataprovider)</t>
+  </si>
+  <si>
+    <t>src\test\java\me\manzhos\tests\AddingComputerHappyPathTest</t>
+  </si>
+  <si>
+    <t>checkIncorrectDiscontinuedDatesAreValidatedTest</t>
+  </si>
+  <si>
+    <t>checkIncorrectIntroductionDatesAreValidatedTest</t>
+  </si>
+  <si>
+    <t>src\test\java\me\manzhos\tests\AddingComputerUnhappyPathTest</t>
+  </si>
+  <si>
+    <t>checkComputerNameIsMandatoryFieldTest</t>
+  </si>
+  <si>
+    <t>1. "Introduced date" field is highlighted with red
+2. "Discontinued date" field is highlighted with red</t>
+  </si>
+  <si>
+    <t>checkBothDatesAreValidatedTest</t>
+  </si>
+  <si>
+    <t>checkCancelButtonDoesntCreateNewRecordTest</t>
   </si>
 </sst>
 </file>
@@ -414,7 +429,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -472,19 +487,6 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -585,23 +587,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -616,6 +615,51 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -625,51 +669,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -953,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -992,13 +992,13 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="29" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="8" t="s">
@@ -1009,9 +1009,9 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="41"/>
-      <c r="B7" s="34"/>
-      <c r="C7" s="42"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="30"/>
       <c r="D7" s="8" t="s">
         <v>16</v>
       </c>
@@ -1020,13 +1020,13 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="29" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="8" t="s">
@@ -1037,9 +1037,9 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="41"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="42"/>
+      <c r="A9" s="26"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="30"/>
       <c r="D9" s="8" t="s">
         <v>18</v>
       </c>
@@ -1048,13 +1048,13 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="29" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="8" t="s">
@@ -1065,9 +1065,9 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="41"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="42"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="30"/>
       <c r="D11" s="8" t="s">
         <v>20</v>
       </c>
@@ -1076,13 +1076,13 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="29" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="8" t="s">
@@ -1093,9 +1093,9 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="43"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="42"/>
+      <c r="A13" s="32"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="30"/>
       <c r="D13" s="4" t="s">
         <v>26</v>
       </c>
@@ -1121,13 +1121,13 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="29" t="s">
         <v>14</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -1139,8 +1139,8 @@
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="39"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="36"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="37"/>
       <c r="D16" s="4" t="s">
         <v>35</v>
       </c>
@@ -1150,8 +1150,8 @@
     </row>
     <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="39"/>
-      <c r="B17" s="33"/>
-      <c r="C17" s="36"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="37"/>
       <c r="D17" s="4" t="s">
         <v>36</v>
       </c>
@@ -1161,8 +1161,8 @@
     </row>
     <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="39"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="36"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="37"/>
       <c r="D18" s="4" t="s">
         <v>37</v>
       </c>
@@ -1172,8 +1172,8 @@
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="39"/>
-      <c r="B19" s="33"/>
-      <c r="C19" s="36"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="37"/>
       <c r="D19" s="4" t="s">
         <v>34</v>
       </c>
@@ -1183,8 +1183,8 @@
     </row>
     <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="39"/>
-      <c r="B20" s="33"/>
-      <c r="C20" s="36"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="37"/>
       <c r="D20" s="4" t="s">
         <v>38</v>
       </c>
@@ -1194,8 +1194,8 @@
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="39"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="36"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="37"/>
       <c r="D21" s="4" t="s">
         <v>39</v>
       </c>
@@ -1205,10 +1205,10 @@
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="39"/>
-      <c r="B22" s="33"/>
-      <c r="C22" s="36"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="37"/>
       <c r="D22" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>53</v>
@@ -1216,10 +1216,10 @@
     </row>
     <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="39"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="36"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="37"/>
       <c r="D23" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>53</v>
@@ -1227,118 +1227,118 @@
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="39"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="36"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="37"/>
       <c r="D24" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="29" t="s">
+      <c r="A25" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="32" t="s">
+      <c r="B25" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="35" t="s">
+      <c r="C25" s="29" t="s">
         <v>14</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="30"/>
-      <c r="B26" s="33"/>
-      <c r="C26" s="36"/>
+      <c r="A26" s="34"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="37"/>
       <c r="D26" s="4" t="s">
         <v>35</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="30"/>
-      <c r="B27" s="33"/>
-      <c r="C27" s="36"/>
+      <c r="A27" s="34"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="37"/>
       <c r="D27" s="4" t="s">
         <v>36</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="30"/>
-      <c r="B28" s="33"/>
-      <c r="C28" s="36"/>
+      <c r="A28" s="34"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="37"/>
       <c r="D28" s="4" t="s">
         <v>37</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="30"/>
-      <c r="B29" s="33"/>
-      <c r="C29" s="36"/>
+      <c r="A29" s="34"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="37"/>
       <c r="D29" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="30"/>
-      <c r="B30" s="33"/>
-      <c r="C30" s="36"/>
+      <c r="A30" s="34"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="37"/>
       <c r="D30" s="4" t="s">
         <v>38</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
-      <c r="B31" s="33"/>
-      <c r="C31" s="36"/>
+      <c r="A31" s="34"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="37"/>
       <c r="D31" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="30"/>
-      <c r="B32" s="33"/>
-      <c r="C32" s="36"/>
+      <c r="A32" s="34"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="37"/>
       <c r="D32" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="31"/>
-      <c r="B33" s="34"/>
-      <c r="C33" s="37"/>
+      <c r="A33" s="35"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="38"/>
       <c r="D33" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1355,7 +1355,7 @@
         <v>51</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>57</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1365,24 +1365,24 @@
       <c r="B35" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="21" t="s">
+      <c r="C35" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D35" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="E35" s="20" t="s">
+      <c r="E35" s="16" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="B36" s="27" t="s">
+      <c r="A36" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="C36" s="28" t="s">
+      <c r="C36" s="42" t="s">
         <v>7</v>
       </c>
       <c r="D36" s="16" t="s">
@@ -1393,95 +1393,95 @@
       </c>
     </row>
     <row r="37" spans="1:5" ht="135" x14ac:dyDescent="0.25">
-      <c r="A37" s="26"/>
-      <c r="B37" s="27"/>
-      <c r="C37" s="28"/>
+      <c r="A37" s="40"/>
+      <c r="B37" s="41"/>
+      <c r="C37" s="42"/>
       <c r="D37" s="16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E37" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A38" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38" s="12" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A38" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="B38" s="12" t="s">
-        <v>62</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E38" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A39" s="26" t="s">
+      <c r="A39" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="B39" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="C39" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B39" s="27" t="s">
+      <c r="E39" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="C39" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="D39" s="16" t="s">
+    </row>
+    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="40"/>
+      <c r="B40" s="41"/>
+      <c r="C40" s="42"/>
+      <c r="D40" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="E39" s="16" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="26"/>
-      <c r="B40" s="27"/>
-      <c r="C40" s="28"/>
-      <c r="D40" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="E40" s="16" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="23"/>
-      <c r="B41" s="24"/>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23"/>
-      <c r="E41" s="23"/>
+      <c r="A41" s="22"/>
+      <c r="B41" s="23"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="22"/>
     </row>
   </sheetData>
   <autoFilter ref="A5:E9"/>
   <mergeCells count="24">
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="A25:A33"/>
+    <mergeCell ref="B25:B33"/>
+    <mergeCell ref="C25:C33"/>
+    <mergeCell ref="A15:A24"/>
+    <mergeCell ref="B15:B24"/>
+    <mergeCell ref="C15:C24"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="A12:A13"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A25:A33"/>
-    <mergeCell ref="B25:B33"/>
-    <mergeCell ref="C25:C33"/>
-    <mergeCell ref="A15:A24"/>
-    <mergeCell ref="B15:B24"/>
-    <mergeCell ref="C15:C24"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
@@ -1496,7 +1496,7 @@
   <dimension ref="C2:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1507,14 +1507,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="24" t="s">
         <v>79</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="E2" s="25" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="3" spans="3:5" x14ac:dyDescent="0.25">
@@ -1522,10 +1522,10 @@
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.25">
@@ -1533,10 +1533,10 @@
         <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.25">
@@ -1544,10 +1544,10 @@
         <v>22</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.25">
@@ -1555,46 +1555,66 @@
         <v>24</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E10" s="43" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" s="43" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
@@ -1605,14 +1625,14 @@
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>

</xml_diff>

<commit_message>
Edit computer happy and unhappy pathes were added
Traceability section of test cases was updated
</commit_message>
<xml_diff>
--- a/ComputerDatabase_TestCases.xlsx
+++ b/ComputerDatabase_TestCases.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="97">
   <si>
     <t>Test Case Id</t>
   </si>
@@ -216,15 +216,6 @@
   </si>
   <si>
     <t>Edit Computer (Happy path)</t>
-  </si>
-  <si>
-    <t>1. Input "My new computer!" to filter field
-2. Click "Filter by name" button
-3. Click computer name in "Computer name" field</t>
-  </si>
-  <si>
-    <t>1. "Edit computer screen" is displayed
-2. "Computer name" field contains "My new computer!" value</t>
   </si>
   <si>
     <t>1. Input "Both dates are validated" to "Computer name" field
@@ -384,6 +375,32 @@
   </si>
   <si>
     <t>checkCancelButtonDoesntCreateNewRecordTest</t>
+  </si>
+  <si>
+    <t>1. Input "@A computer again@" to filter field
+2. Click "Filter by name" button
+3. Click computer name in "Computer name" field</t>
+  </si>
+  <si>
+    <t>1. Application URL is opened
+2. "Add a new computer" button is clicked
+3. New computer with name "@A computer again@" is created</t>
+  </si>
+  <si>
+    <t>1. "Edit computer screen" is displayed
+2. "Computer name" field contains "@A computer again@" value</t>
+  </si>
+  <si>
+    <t>editComputerByPopulatedAllFieldsTest</t>
+  </si>
+  <si>
+    <t>src\test\java\me\manzhos\tests\EditComputerHappyPath</t>
+  </si>
+  <si>
+    <t>cancelEditingExistingComputerDataTest</t>
+  </si>
+  <si>
+    <t>src\test\java\me\manzhos\tests\EditComputerUnhappyPath.java</t>
   </si>
 </sst>
 </file>
@@ -545,7 +562,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -615,61 +632,68 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -954,7 +978,7 @@
   <dimension ref="A2:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -992,13 +1016,13 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="35" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="8" t="s">
@@ -1009,9 +1033,9 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="30"/>
+      <c r="A7" s="41"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="42"/>
       <c r="D7" s="8" t="s">
         <v>16</v>
       </c>
@@ -1020,13 +1044,13 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="35" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="8" t="s">
@@ -1037,9 +1061,9 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="30"/>
+      <c r="A9" s="41"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="42"/>
       <c r="D9" s="8" t="s">
         <v>18</v>
       </c>
@@ -1048,13 +1072,13 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="35" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="8" t="s">
@@ -1065,9 +1089,9 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="30"/>
+      <c r="A11" s="41"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="42"/>
       <c r="D11" s="8" t="s">
         <v>20</v>
       </c>
@@ -1076,13 +1100,13 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="35" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="8" t="s">
@@ -1093,9 +1117,9 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="30"/>
+      <c r="A13" s="43"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="42"/>
       <c r="D13" s="4" t="s">
         <v>26</v>
       </c>
@@ -1117,228 +1141,228 @@
         <v>32</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="35" t="s">
         <v>14</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>33</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="39"/>
-      <c r="B16" s="36"/>
-      <c r="C16" s="37"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="36"/>
       <c r="D16" s="4" t="s">
         <v>35</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="39"/>
-      <c r="B17" s="36"/>
-      <c r="C17" s="37"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="36"/>
       <c r="D17" s="4" t="s">
         <v>36</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="39"/>
-      <c r="B18" s="36"/>
-      <c r="C18" s="37"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="36"/>
       <c r="D18" s="4" t="s">
         <v>37</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="39"/>
-      <c r="B19" s="36"/>
-      <c r="C19" s="37"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="36"/>
       <c r="D19" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="39"/>
-      <c r="B20" s="36"/>
-      <c r="C20" s="37"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="36"/>
       <c r="D20" s="4" t="s">
         <v>38</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="39"/>
-      <c r="B21" s="36"/>
-      <c r="C21" s="37"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="36"/>
       <c r="D21" s="4" t="s">
         <v>39</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="39"/>
-      <c r="B22" s="36"/>
-      <c r="C22" s="37"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="36"/>
       <c r="D22" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="39"/>
-      <c r="B23" s="36"/>
-      <c r="C23" s="37"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="36"/>
       <c r="D23" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="39"/>
-      <c r="B24" s="36"/>
-      <c r="C24" s="37"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="36"/>
       <c r="D24" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E24" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="34"/>
-      <c r="B26" s="36"/>
-      <c r="C26" s="37"/>
+      <c r="A26" s="30"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="36"/>
       <c r="D26" s="4" t="s">
         <v>35</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="34"/>
-      <c r="B27" s="36"/>
-      <c r="C27" s="37"/>
+      <c r="A27" s="30"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="36"/>
       <c r="D27" s="4" t="s">
         <v>36</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="34"/>
-      <c r="B28" s="36"/>
-      <c r="C28" s="37"/>
+      <c r="A28" s="30"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="36"/>
       <c r="D28" s="4" t="s">
         <v>37</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="34"/>
-      <c r="B29" s="36"/>
-      <c r="C29" s="37"/>
+      <c r="A29" s="30"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="36"/>
       <c r="D29" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="34"/>
-      <c r="B30" s="36"/>
-      <c r="C30" s="37"/>
+      <c r="A30" s="30"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="36"/>
       <c r="D30" s="4" t="s">
         <v>38</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="34"/>
-      <c r="B31" s="36"/>
-      <c r="C31" s="37"/>
+      <c r="A31" s="30"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="36"/>
       <c r="D31" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="34"/>
-      <c r="B32" s="36"/>
-      <c r="C32" s="37"/>
+      <c r="A32" s="30"/>
+      <c r="B32" s="33"/>
+      <c r="C32" s="36"/>
       <c r="D32" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="35"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="38"/>
+      <c r="A33" s="31"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="37"/>
       <c r="D33" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1352,10 +1376,10 @@
         <v>14</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1376,73 +1400,73 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="40" t="s">
-        <v>70</v>
-      </c>
-      <c r="B36" s="41" t="s">
+      <c r="A36" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="B36" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="C36" s="42" t="s">
-        <v>7</v>
+      <c r="C36" s="45" t="s">
+        <v>91</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>50</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="135" x14ac:dyDescent="0.25">
-      <c r="A37" s="40"/>
-      <c r="B37" s="41"/>
-      <c r="C37" s="42"/>
+      <c r="A37" s="26"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="46"/>
       <c r="D37" s="16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A38" s="21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E38" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A39" s="40" t="s">
+      <c r="A39" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C39" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="B39" s="41" t="s">
+      <c r="E39" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="C39" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="D39" s="16" t="s">
+    </row>
+    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="26"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="E39" s="16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="40"/>
-      <c r="B40" s="41"/>
-      <c r="C40" s="42"/>
-      <c r="D40" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="E40" s="16" t="s">
         <v>46</v>
@@ -1458,30 +1482,30 @@
   </sheetData>
   <autoFilter ref="A5:E9"/>
   <mergeCells count="24">
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A25:A33"/>
+    <mergeCell ref="B25:B33"/>
+    <mergeCell ref="C25:C33"/>
+    <mergeCell ref="A15:A24"/>
+    <mergeCell ref="B15:B24"/>
+    <mergeCell ref="C15:C24"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="C39:C40"/>
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="B36:B37"/>
     <mergeCell ref="C36:C37"/>
-    <mergeCell ref="A25:A33"/>
-    <mergeCell ref="B25:B33"/>
-    <mergeCell ref="C25:C33"/>
-    <mergeCell ref="A15:A24"/>
-    <mergeCell ref="B15:B24"/>
-    <mergeCell ref="C15:C24"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="A8:A9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
@@ -1496,7 +1520,7 @@
   <dimension ref="C2:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1508,13 +1532,13 @@
   <sheetData>
     <row r="2" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C2" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" s="24" t="s">
         <v>77</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" s="24" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="3" spans="3:5" x14ac:dyDescent="0.25">
@@ -1522,10 +1546,10 @@
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.25">
@@ -1533,10 +1557,10 @@
         <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.25">
@@ -1544,10 +1568,10 @@
         <v>22</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.25">
@@ -1555,10 +1579,10 @@
         <v>24</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.25">
@@ -1566,10 +1590,10 @@
         <v>28</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.25">
@@ -1577,10 +1601,10 @@
         <v>40</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.25">
@@ -1588,10 +1612,10 @@
         <v>41</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.25">
@@ -1599,10 +1623,10 @@
         <v>42</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E10" s="43" t="s">
-        <v>90</v>
+        <v>85</v>
+      </c>
+      <c r="E10" s="44" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.25">
@@ -1610,29 +1634,37 @@
         <v>43</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E11" s="43" t="s">
-        <v>91</v>
+        <v>82</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+        <v>57</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>

</xml_diff>

<commit_message>
Deletion test was added
Edition calsses names were updated
</commit_message>
<xml_diff>
--- a/ComputerDatabase_TestCases.xlsx
+++ b/ComputerDatabase_TestCases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Manual test cases" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="99">
   <si>
     <t>Test Case Id</t>
   </si>
@@ -400,7 +400,13 @@
     <t>cancelEditingExistingComputerDataTest</t>
   </si>
   <si>
-    <t>src\test\java\me\manzhos\tests\EditComputerUnhappyPath.java</t>
+    <t>removeComputerTest</t>
+  </si>
+  <si>
+    <t>src\test\java\me\manzhos\tests\EditComputerUnhappyPath</t>
+  </si>
+  <si>
+    <t>src\test\java\me\manzhos\tests\DeleteComputerTest.java</t>
   </si>
 </sst>
 </file>
@@ -633,6 +639,52 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -642,52 +694,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -977,7 +983,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
@@ -1016,13 +1022,13 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="31" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="8" t="s">
@@ -1033,9 +1039,9 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="41"/>
-      <c r="B7" s="34"/>
-      <c r="C7" s="42"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="32"/>
       <c r="D7" s="8" t="s">
         <v>16</v>
       </c>
@@ -1044,13 +1050,13 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="31" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="8" t="s">
@@ -1061,9 +1067,9 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="41"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="42"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="32"/>
       <c r="D9" s="8" t="s">
         <v>18</v>
       </c>
@@ -1072,13 +1078,13 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="31" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="8" t="s">
@@ -1089,9 +1095,9 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="41"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="42"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="32"/>
       <c r="D11" s="8" t="s">
         <v>20</v>
       </c>
@@ -1100,13 +1106,13 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="31" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="8" t="s">
@@ -1117,9 +1123,9 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="43"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="42"/>
+      <c r="A13" s="34"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="32"/>
       <c r="D13" s="4" t="s">
         <v>26</v>
       </c>
@@ -1145,13 +1151,13 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="31" t="s">
         <v>14</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -1162,9 +1168,9 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="39"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="36"/>
+      <c r="A16" s="41"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="39"/>
       <c r="D16" s="4" t="s">
         <v>35</v>
       </c>
@@ -1173,9 +1179,9 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="39"/>
-      <c r="B17" s="33"/>
-      <c r="C17" s="36"/>
+      <c r="A17" s="41"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="39"/>
       <c r="D17" s="4" t="s">
         <v>36</v>
       </c>
@@ -1184,9 +1190,9 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="39"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="36"/>
+      <c r="A18" s="41"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="39"/>
       <c r="D18" s="4" t="s">
         <v>37</v>
       </c>
@@ -1195,9 +1201,9 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="39"/>
-      <c r="B19" s="33"/>
-      <c r="C19" s="36"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="39"/>
       <c r="D19" s="4" t="s">
         <v>34</v>
       </c>
@@ -1206,9 +1212,9 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="39"/>
-      <c r="B20" s="33"/>
-      <c r="C20" s="36"/>
+      <c r="A20" s="41"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="39"/>
       <c r="D20" s="4" t="s">
         <v>38</v>
       </c>
@@ -1217,9 +1223,9 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="39"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="36"/>
+      <c r="A21" s="41"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="39"/>
       <c r="D21" s="4" t="s">
         <v>39</v>
       </c>
@@ -1228,9 +1234,9 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="39"/>
-      <c r="B22" s="33"/>
-      <c r="C22" s="36"/>
+      <c r="A22" s="41"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="39"/>
       <c r="D22" s="4" t="s">
         <v>61</v>
       </c>
@@ -1239,9 +1245,9 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="39"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="36"/>
+      <c r="A23" s="41"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="39"/>
       <c r="D23" s="4" t="s">
         <v>62</v>
       </c>
@@ -1250,9 +1256,9 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="39"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="36"/>
+      <c r="A24" s="41"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="39"/>
       <c r="D24" s="4" t="s">
         <v>64</v>
       </c>
@@ -1261,13 +1267,13 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="29" t="s">
+      <c r="A25" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="32" t="s">
+      <c r="B25" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="35" t="s">
+      <c r="C25" s="31" t="s">
         <v>14</v>
       </c>
       <c r="D25" s="4" t="s">
@@ -1278,9 +1284,9 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="30"/>
-      <c r="B26" s="33"/>
-      <c r="C26" s="36"/>
+      <c r="A26" s="36"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="39"/>
       <c r="D26" s="4" t="s">
         <v>35</v>
       </c>
@@ -1289,9 +1295,9 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="30"/>
-      <c r="B27" s="33"/>
-      <c r="C27" s="36"/>
+      <c r="A27" s="36"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="39"/>
       <c r="D27" s="4" t="s">
         <v>36</v>
       </c>
@@ -1300,9 +1306,9 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="30"/>
-      <c r="B28" s="33"/>
-      <c r="C28" s="36"/>
+      <c r="A28" s="36"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="39"/>
       <c r="D28" s="4" t="s">
         <v>37</v>
       </c>
@@ -1311,9 +1317,9 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="30"/>
-      <c r="B29" s="33"/>
-      <c r="C29" s="36"/>
+      <c r="A29" s="36"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="39"/>
       <c r="D29" s="4" t="s">
         <v>34</v>
       </c>
@@ -1322,9 +1328,9 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="30"/>
-      <c r="B30" s="33"/>
-      <c r="C30" s="36"/>
+      <c r="A30" s="36"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="39"/>
       <c r="D30" s="4" t="s">
         <v>38</v>
       </c>
@@ -1333,9 +1339,9 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
-      <c r="B31" s="33"/>
-      <c r="C31" s="36"/>
+      <c r="A31" s="36"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="39"/>
       <c r="D31" s="4" t="s">
         <v>65</v>
       </c>
@@ -1344,9 +1350,9 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="30"/>
-      <c r="B32" s="33"/>
-      <c r="C32" s="36"/>
+      <c r="A32" s="36"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="39"/>
       <c r="D32" s="4" t="s">
         <v>66</v>
       </c>
@@ -1355,9 +1361,9 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="31"/>
-      <c r="B33" s="34"/>
-      <c r="C33" s="37"/>
+      <c r="A33" s="37"/>
+      <c r="B33" s="30"/>
+      <c r="C33" s="40"/>
       <c r="D33" s="4" t="s">
         <v>63</v>
       </c>
@@ -1400,10 +1406,10 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="26" t="s">
+      <c r="A36" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="B36" s="27" t="s">
+      <c r="B36" s="43" t="s">
         <v>48</v>
       </c>
       <c r="C36" s="45" t="s">
@@ -1417,8 +1423,8 @@
       </c>
     </row>
     <row r="37" spans="1:5" ht="135" x14ac:dyDescent="0.25">
-      <c r="A37" s="26"/>
-      <c r="B37" s="27"/>
+      <c r="A37" s="42"/>
+      <c r="B37" s="43"/>
       <c r="C37" s="46"/>
       <c r="D37" s="16" t="s">
         <v>55</v>
@@ -1445,13 +1451,13 @@
       </c>
     </row>
     <row r="39" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A39" s="26" t="s">
+      <c r="A39" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="B39" s="27" t="s">
+      <c r="B39" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C39" s="28" t="s">
+      <c r="C39" s="44" t="s">
         <v>7</v>
       </c>
       <c r="D39" s="16" t="s">
@@ -1462,9 +1468,9 @@
       </c>
     </row>
     <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="26"/>
-      <c r="B40" s="27"/>
-      <c r="C40" s="28"/>
+      <c r="A40" s="42"/>
+      <c r="B40" s="43"/>
+      <c r="C40" s="44"/>
       <c r="D40" s="2" t="s">
         <v>74</v>
       </c>
@@ -1482,30 +1488,30 @@
   </sheetData>
   <autoFilter ref="A5:E9"/>
   <mergeCells count="24">
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="A25:A33"/>
+    <mergeCell ref="B25:B33"/>
+    <mergeCell ref="C25:C33"/>
+    <mergeCell ref="A15:A24"/>
+    <mergeCell ref="B15:B24"/>
+    <mergeCell ref="C15:C24"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="A12:A13"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A25:A33"/>
-    <mergeCell ref="B25:B33"/>
-    <mergeCell ref="C25:C33"/>
-    <mergeCell ref="A15:A24"/>
-    <mergeCell ref="B15:B24"/>
-    <mergeCell ref="C15:C24"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
@@ -1519,8 +1525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1625,7 +1631,7 @@
       <c r="D10" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E10" s="44" t="s">
+      <c r="E10" s="26" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1656,7 +1662,7 @@
         <v>57</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>95</v>
@@ -1666,8 +1672,12 @@
       <c r="C14" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="D14" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>96</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>